<commit_message>
chore: Set tolerance to 0.4
</commit_message>
<xml_diff>
--- a/io/input/tutorial_03_methionine_cycle.xlsx
+++ b/io/input/tutorial_03_methionine_cycle.xlsx
@@ -710,7 +710,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12:C16"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -805,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -829,7 +829,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -853,7 +853,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K35" activeCellId="1" sqref="C12:C16 K35"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2084,7 +2084,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2985,7 +2985,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3275,7 +3275,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="C12:C16 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3442,7 +3442,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3606,7 +3606,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C12:C16 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3756,7 +3756,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C12:C16 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3918,7 +3918,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="C12:C16 F20"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4201,7 +4201,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C12:C16"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>